<commit_message>
Add list for refrigerator moves
</commit_message>
<xml_diff>
--- a/app/config/tables/refrigerator_moves/forms/refrigerator_moves/refrigerator_moves.xlsx
+++ b/app/config/tables/refrigerator_moves/forms/refrigerator_moves/refrigerator_moves.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="37940" windowHeight="19700" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="5" r:id="rId3"/>
+    <sheet name="properties" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="72">
   <si>
     <t>comments</t>
   </si>
@@ -168,6 +169,75 @@
   </si>
   <si>
     <t>new_facility_id</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>aspect</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>defaultViewType</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>detailViewFileName</t>
+  </si>
+  <si>
+    <t>listViewFileName</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>unverifiedUserCanCreate</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>defaultAccessOnCreation</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
+  </si>
+  <si>
+    <t>FormType</t>
+  </si>
+  <si>
+    <t>FormType.formType</t>
+  </si>
+  <si>
+    <t>SURVEY</t>
+  </si>
+  <si>
+    <t>SurveyUtil</t>
+  </si>
+  <si>
+    <t>SurveyUtil.formId</t>
+  </si>
+  <si>
+    <t>wrong_form</t>
+  </si>
+  <si>
+    <t>config/tables/refrigerator_moves/html/refrigerator_moves_detail.html</t>
+  </si>
+  <si>
+    <t>config/tables/refrigerator_moves/html/refrigerator_moves_list.html</t>
   </si>
 </sst>
 </file>
@@ -248,7 +318,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -281,6 +351,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -696,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
@@ -1030,4 +1105,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="22"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>